<commit_message>
complete import subject and fix ui adminheader
</commit_message>
<xml_diff>
--- a/import/import_mon.xlsx
+++ b/import/import_mon.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\L A P T R I N H V I EN WEBSITE\Cd2\nckh_ng\import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65944162-E30F-4B32-A84C-51FC4111D7B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C18B7CD-6FB9-48CA-9D3D-9B0008B48F5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BCF34E21-58DF-44CD-BC56-38C631FFAE60}"/>
   </bookViews>
@@ -53,16 +53,16 @@
     <t>cd1</t>
   </si>
   <si>
-    <t>Công nghệ thông tin</t>
-  </si>
-  <si>
     <t>A1</t>
   </si>
   <si>
     <t>a1</t>
   </si>
   <si>
-    <t>Thiết kế đồ họa</t>
+    <t>CNTT</t>
+  </si>
+  <si>
+    <t>DH</t>
   </si>
 </sst>
 </file>
@@ -460,7 +460,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -489,15 +489,15 @@
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>7</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>8</v>

</xml_diff>